<commit_message>
Update results with 6 lagacy stations
</commit_message>
<xml_diff>
--- a/results/scenario_1/scenario_1.xlsx
+++ b/results/scenario_1/scenario_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MetodySymulacyjne\MS_project2\results\scenario_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{394955C6-F538-4053-8357-66343A311ADC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466DD19C-79FC-4040-8FB7-714D46876B29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{303A26E9-D629-421F-BDB8-B96358A3F3B8}"/>
+    <workbookView xWindow="7815" yWindow="1620" windowWidth="17940" windowHeight="9210" xr2:uid="{303A26E9-D629-421F-BDB8-B96358A3F3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_1" sheetId="1" r:id="rId1"/>
@@ -1611,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F634F3-CA75-4E29-820E-C70316CED6F2}">
   <dimension ref="B2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add new versions of scripts, new results added
</commit_message>
<xml_diff>
--- a/results/scenario_1/scenario_1.xlsx
+++ b/results/scenario_1/scenario_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MetodySymulacyjne\MS_project2\results\scenario_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449498FF-5900-488C-87A0-C8ED4C36BEB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4C898B-204C-48EB-8B81-D2F38314D383}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23554" yWindow="-6523" windowWidth="23657" windowHeight="15840" xr2:uid="{303A26E9-D629-421F-BDB8-B96358A3F3B8}"/>
+    <workbookView xWindow="-69" yWindow="-69" windowWidth="23589" windowHeight="15772" xr2:uid="{303A26E9-D629-421F-BDB8-B96358A3F3B8}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_1" sheetId="1" r:id="rId1"/>
@@ -1612,7 +1612,7 @@
   <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>